<commit_message>
update In Class Demonstrations
</commit_message>
<xml_diff>
--- a/Projects/Federal Reserve Data/$pi$Disaggregated C&A  Diff-in-DiffDAGVAR 2010-01-31 to 2020-02-29.xlsx
+++ b/Projects/Federal Reserve Data/$pi$Disaggregated C&A  Diff-in-DiffDAGVAR 2010-01-31 to 2020-02-29.xlsx
@@ -14,42 +14,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>$\pi$</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
     <t>$\pi$ Lag</t>
   </si>
   <si>
+    <t>A Lag</t>
+  </si>
+  <si>
     <t>C Lag</t>
   </si>
   <si>
-    <t>Constant</t>
-  </si>
-  <si>
-    <t>r2_adj</t>
-  </si>
-  <si>
-    <t>-0.693***</t>
-  </si>
-  <si>
-    <t>0.004</t>
-  </si>
-  <si>
-    <t>0.123*</t>
-  </si>
-  <si>
-    <t>0.889*</t>
-  </si>
-  <si>
-    <t>-0.605***</t>
-  </si>
-  <si>
-    <t>-0.867**</t>
+    <t>-0.636***</t>
+  </si>
+  <si>
+    <t>0.202</t>
+  </si>
+  <si>
+    <t>-0.013</t>
+  </si>
+  <si>
+    <t>-0.071</t>
+  </si>
+  <si>
+    <t>-0.412***</t>
+  </si>
+  <si>
+    <t>-0.052***</t>
+  </si>
+  <si>
+    <t>1.118**</t>
+  </si>
+  <si>
+    <t>1.004</t>
+  </si>
+  <si>
+    <t>-0.698***</t>
   </si>
 </sst>
 </file>
@@ -407,23 +416,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -431,10 +443,13 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -442,10 +457,13 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -453,16 +471,8 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0.59</v>
-      </c>
-      <c r="C5">
-        <v>0.67</v>
+      <c r="D4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>